<commit_message>
changed some HTML and styling
</commit_message>
<xml_diff>
--- a/js/links.xlsx
+++ b/js/links.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="211">
   <si>
     <t>Timestamp</t>
   </si>
@@ -193,7 +193,7 @@
     <t>https://github.com/JYumek/Roots-let-s-start-Dev-ing-.git</t>
   </si>
   <si>
-    <t>https://github.com/JYumek/Roots-let-s-start-Dev-ing-/blob/1618e6ef02c0a112006f0817539481393a9aab9d/links.html</t>
+    <t>https://jyumek.github.io/Let-s-start-Dev-ing-/</t>
   </si>
   <si>
     <t>C S Sonali</t>
@@ -370,12 +370,12 @@
     <t>Hopeless Engineer's</t>
   </si>
   <si>
+    <t>https://github.com/Sinchana1706</t>
+  </si>
+  <si>
     <t>https://sinchana1706.github.io/linktree/</t>
   </si>
   <si>
-    <t>https://github.com/Sinchana1706</t>
-  </si>
-  <si>
     <t>Sinchana.M</t>
   </si>
   <si>
@@ -575,6 +575,75 @@
   </si>
   <si>
     <t>Suhasravi2002@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Amigos </t>
+  </si>
+  <si>
+    <t>https://github.com/sandeepraor</t>
+  </si>
+  <si>
+    <t>https://sandeepraor.github.io/link-tree/</t>
+  </si>
+  <si>
+    <t>Sandeep Rao R</t>
+  </si>
+  <si>
+    <t>sandeepr062003@gmail.com</t>
+  </si>
+  <si>
+    <t>SRP</t>
+  </si>
+  <si>
+    <t>https://github.com/sankethrajpatil</t>
+  </si>
+  <si>
+    <t>https://sankethrajpatil.github.io/LinkTree/</t>
+  </si>
+  <si>
+    <t>Sanketh Rajshekhar Patil</t>
+  </si>
+  <si>
+    <t>sankethrajpatil@ieee.org</t>
+  </si>
+  <si>
+    <t>Justme</t>
+  </si>
+  <si>
+    <t>https://sam1429.github.io/Linktree/</t>
+  </si>
+  <si>
+    <t>Samyuktha Sridhar</t>
+  </si>
+  <si>
+    <t>samyuktha.sridhar.2014@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhishek </t>
+  </si>
+  <si>
+    <t>https://github.com/Abhishek-K-N?tab=repositories</t>
+  </si>
+  <si>
+    <t>https://abhishek-k-n.github.io/linktree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhishek KN </t>
+  </si>
+  <si>
+    <t>knabhishek02@gmail.com</t>
+  </si>
+  <si>
+    <t>Debarun Das</t>
+  </si>
+  <si>
+    <t>https://github.com/debarundas1999/debarunsLinktre</t>
+  </si>
+  <si>
+    <t>https://debarundas1999.github.io/debarunsLinktre/</t>
+  </si>
+  <si>
+    <t>das.debarun912210@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -596,11 +665,11 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF1155CC"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -853,7 +922,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="21.57"/>
+    <col customWidth="1" min="1" max="2" width="21.57"/>
+    <col customWidth="1" min="3" max="3" width="27.57"/>
+    <col customWidth="1" min="4" max="4" width="46.29"/>
+    <col customWidth="1" min="5" max="25" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -925,7 +997,7 @@
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -951,10 +1023,10 @@
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -980,10 +1052,10 @@
       <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1009,10 +1081,10 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1038,7 +1110,7 @@
       <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1085,10 +1157,10 @@
       <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1114,10 +1186,10 @@
       <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1143,10 +1215,10 @@
       <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1201,10 +1273,10 @@
       <c r="B11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1230,10 +1302,10 @@
       <c r="B12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1274,10 +1346,10 @@
       <c r="B13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1303,10 +1375,10 @@
       <c r="B14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1332,10 +1404,10 @@
       <c r="B15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>87</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1361,10 +1433,10 @@
       <c r="B16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>92</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1390,10 +1462,10 @@
       <c r="B17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1419,10 +1491,10 @@
       <c r="B18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>101</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1451,7 +1523,7 @@
       <c r="C19" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>106</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1477,10 +1549,10 @@
       <c r="B20" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1506,10 +1578,10 @@
       <c r="B21" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>116</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1594,10 +1666,10 @@
       <c r="B23" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>129</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1623,10 +1695,10 @@
       <c r="B24" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1652,10 +1724,10 @@
       <c r="B25" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>139</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1681,10 +1753,10 @@
       <c r="B26" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1710,10 +1782,10 @@
       <c r="B27" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>149</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1754,10 +1826,10 @@
       <c r="B28" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>157</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1783,10 +1855,10 @@
       <c r="B29" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>163</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1812,10 +1884,10 @@
       <c r="B30" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -1841,10 +1913,10 @@
       <c r="B31" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1870,10 +1942,10 @@
       <c r="B32" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>178</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1899,10 +1971,10 @@
       <c r="B33" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>149</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1943,10 +2015,10 @@
       <c r="B34" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1963,6 +2035,151 @@
       </c>
       <c r="I34" s="3" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <v>44457.9551187037</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G35" s="3">
+        <v>8.660781172E9</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2">
+        <v>44457.98313966436</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G36" s="3">
+        <v>9.611650218E9</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2">
+        <v>44458.02364275463</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G37" s="3">
+        <v>9.108562257E9</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2">
+        <v>44458.334797013886</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G38" s="3">
+        <v>9.482031933E9</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2">
+        <v>44458.598336863426</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G39" s="3">
+        <v>8.787810486E9</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2033,7 +2250,17 @@
     <hyperlink r:id="rId64" ref="D33"/>
     <hyperlink r:id="rId65" ref="C34"/>
     <hyperlink r:id="rId66" ref="D34"/>
+    <hyperlink r:id="rId67" ref="C35"/>
+    <hyperlink r:id="rId68" ref="D35"/>
+    <hyperlink r:id="rId69" ref="C36"/>
+    <hyperlink r:id="rId70" ref="D36"/>
+    <hyperlink r:id="rId71" ref="C37"/>
+    <hyperlink r:id="rId72" ref="D37"/>
+    <hyperlink r:id="rId73" ref="C38"/>
+    <hyperlink r:id="rId74" ref="D38"/>
+    <hyperlink r:id="rId75" ref="C39"/>
+    <hyperlink r:id="rId76" ref="D39"/>
   </hyperlinks>
-  <drawing r:id="rId67"/>
+  <drawing r:id="rId77"/>
 </worksheet>
 </file>
</xml_diff>